<commit_message>
#Refactoring classe Player.java #Player reso sottoclasse di Entity.java
</commit_message>
<xml_diff>
--- a/Revisione/Backlog.xlsx
+++ b/Revisione/Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Progetti\FlagV2\Revisione\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B6CCACE-E5CD-4DB7-A7B5-847C5B672F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9E4D2D-1006-44C3-8DBC-5E3D0F4BFDBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flag_2023-12-16_10.56pm" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="114">
   <si>
     <t>Status</t>
   </si>
@@ -388,12 +388,15 @@
   <si>
     <t xml:space="preserve">All' inizio del gioco deve essere mostrata una finestra di dialogo che mostri I comandi di gioco </t>
   </si>
+  <si>
+    <t>20/11/2023-18/12/2023</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,6 +570,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1663,9 +1674,6 @@
     <xf numFmtId="49" fontId="16" fillId="38" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="35" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="18" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2164,50 +2172,53 @@
     <xf numFmtId="49" fontId="0" fillId="36" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="24" fillId="35" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Calcolo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cella collegata" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Cella da controllare" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Colore 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Colore 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Colore 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Colore 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Colore 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Colore 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Neutrale" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Testo avviso" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Testo descrittivo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titolo" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titolo 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titolo 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titolo 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titolo 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Totale" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Valore non valido" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Valore valido" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2230,7 +2241,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2527,7 +2538,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="it-IT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2563,7 +2574,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1288586879"/>
@@ -2621,7 +2632,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="532661231"/>
@@ -2662,7 +2673,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2710,7 +2721,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="it-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3299,9 +3310,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3339,7 +3350,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3445,7 +3456,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3587,7 +3598,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3597,8 +3608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A64" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H87" sqref="H87"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3616,34 +3627,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="107" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="137" t="s">
+      <c r="B1" s="136" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="109"/>
+      <c r="C1" s="115" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="108"/>
     </row>
     <row r="2" spans="1:11" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="123" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="136" t="s">
+      <c r="B2" s="135" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="121" t="s">
+      <c r="C2" s="120" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="119" t="s">
+      <c r="D2" s="118" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="119" t="s">
+      <c r="E2" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="115" t="s">
+      <c r="F2" s="114" t="s">
         <v>58</v>
       </c>
       <c r="H2" s="1"/>
@@ -3652,535 +3665,535 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" s="4" customFormat="1" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="110">
+      <c r="A3" s="109">
         <v>1</v>
       </c>
-      <c r="B3" s="135" t="s">
+      <c r="B3" s="134" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="111" t="s">
+      <c r="C3" s="110" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="112">
-        <v>3</v>
-      </c>
-      <c r="E3" s="113"/>
-      <c r="F3" s="114">
+      <c r="D3" s="111">
+        <v>3</v>
+      </c>
+      <c r="E3" s="112"/>
+      <c r="F3" s="113">
         <f>SUM(F4:F9)</f>
         <v>5</v>
       </c>
-      <c r="G3" s="74"/>
+      <c r="G3" s="73"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="96"/>
-      <c r="B4" s="180"/>
-      <c r="C4" s="24" t="s">
+      <c r="A4" s="95"/>
+      <c r="B4" s="179"/>
+      <c r="C4" s="192" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="55"/>
+      <c r="D4" s="54"/>
       <c r="E4" s="22" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="21">
         <v>2</v>
       </c>
-      <c r="G4" s="75"/>
+      <c r="G4" s="74"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="96"/>
-      <c r="B5" s="181"/>
-      <c r="C5" s="25" t="s">
+      <c r="A5" s="95"/>
+      <c r="B5" s="180"/>
+      <c r="C5" s="24" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="55">
+      <c r="F5" s="54">
         <v>1</v>
       </c>
-      <c r="G5" s="75"/>
+      <c r="G5" s="74"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="96"/>
-      <c r="B6" s="181"/>
-      <c r="C6" s="70" t="s">
+      <c r="A6" s="95"/>
+      <c r="B6" s="180"/>
+      <c r="C6" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="71"/>
+      <c r="D6" s="70"/>
       <c r="E6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="55"/>
-      <c r="G6" s="75"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="74"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="96"/>
-      <c r="B7" s="181"/>
-      <c r="C7" s="25" t="s">
+      <c r="A7" s="95"/>
+      <c r="B7" s="180"/>
+      <c r="C7" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="69"/>
-      <c r="E7" s="72" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="69">
+      <c r="D7" s="68"/>
+      <c r="E7" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="68">
         <v>2</v>
       </c>
-      <c r="G7" s="75"/>
+      <c r="G7" s="74"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="96"/>
-      <c r="B8" s="181"/>
-      <c r="C8" s="25" t="s">
+      <c r="A8" s="95"/>
+      <c r="B8" s="180"/>
+      <c r="C8" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="69"/>
-      <c r="E8" s="72" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="69"/>
-      <c r="G8" s="75"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="68"/>
+      <c r="G8" s="74"/>
     </row>
     <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="96"/>
-      <c r="B9" s="182"/>
-      <c r="C9" s="70" t="s">
+      <c r="A9" s="95"/>
+      <c r="B9" s="181"/>
+      <c r="C9" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="71"/>
+      <c r="D9" s="70"/>
       <c r="E9" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="79"/>
+      <c r="F9" s="78"/>
     </row>
     <row r="10" spans="1:11" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="97">
+      <c r="A10" s="96">
         <v>2</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="27">
         <v>8</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="73">
+      <c r="E10" s="27"/>
+      <c r="F10" s="72">
         <f>SUM(F11:F19)</f>
         <v>9</v>
       </c>
-      <c r="G10" s="74"/>
+      <c r="G10" s="73"/>
     </row>
     <row r="11" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="98"/>
-      <c r="B11" s="183" t="s">
+      <c r="A11" s="97"/>
+      <c r="B11" s="182" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="76">
-        <v>3</v>
-      </c>
-      <c r="G11" s="75"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="75">
+        <v>3</v>
+      </c>
+      <c r="G11" s="74"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="98"/>
-      <c r="B12" s="184"/>
+      <c r="A12" s="97"/>
+      <c r="B12" s="183"/>
       <c r="C12" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="31"/>
+      <c r="D12" s="30"/>
       <c r="E12" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="77">
+      <c r="F12" s="76">
         <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="98"/>
-      <c r="B13" s="184"/>
+      <c r="A13" s="97"/>
+      <c r="B13" s="183"/>
       <c r="C13" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="77">
+      <c r="D13" s="37"/>
+      <c r="E13" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="76">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="98"/>
-      <c r="B14" s="184"/>
+      <c r="A14" s="97"/>
+      <c r="B14" s="183"/>
       <c r="C14" s="18" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="17"/>
-      <c r="E14" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="77">
+      <c r="E14" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="76">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="98"/>
-      <c r="B15" s="184"/>
+      <c r="A15" s="97"/>
+      <c r="B15" s="183"/>
       <c r="C15" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="77">
+      <c r="D15" s="33"/>
+      <c r="E15" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="76">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="98"/>
-      <c r="B16" s="184"/>
+      <c r="A16" s="97"/>
+      <c r="B16" s="183"/>
       <c r="C16" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="77">
+      <c r="D16" s="33"/>
+      <c r="E16" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="76">
         <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="98"/>
-      <c r="B17" s="184"/>
+      <c r="A17" s="97"/>
+      <c r="B17" s="183"/>
       <c r="C17" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="31"/>
+      <c r="D17" s="30"/>
       <c r="E17" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="77">
+      <c r="F17" s="76">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="98"/>
-      <c r="B18" s="184"/>
+      <c r="A18" s="97"/>
+      <c r="B18" s="183"/>
       <c r="C18" s="18" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="17"/>
-      <c r="E18" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="77">
+      <c r="E18" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="76">
         <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="128"/>
-      <c r="B19" s="185"/>
+      <c r="A19" s="127"/>
+      <c r="B19" s="184"/>
       <c r="C19" s="18" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="17"/>
-      <c r="E19" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" s="77">
+      <c r="E19" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="76">
         <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="95">
-        <v>3</v>
-      </c>
-      <c r="B20" s="68" t="s">
+      <c r="A20" s="94">
+        <v>3</v>
+      </c>
+      <c r="B20" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="44">
+      <c r="D20" s="43">
         <v>5</v>
       </c>
-      <c r="E20" s="44"/>
-      <c r="F20" s="87">
+      <c r="E20" s="43"/>
+      <c r="F20" s="86">
         <f>SUM(F21:F26)</f>
         <v>9.5</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="100"/>
-      <c r="B21" s="186" t="s">
+      <c r="A21" s="99"/>
+      <c r="B21" s="185" t="s">
         <v>70</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="47"/>
+      <c r="D21" s="46"/>
       <c r="E21" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="81">
+      <c r="F21" s="80">
         <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="100"/>
-      <c r="B22" s="187"/>
-      <c r="C22" s="41" t="s">
+      <c r="A22" s="99"/>
+      <c r="B22" s="186"/>
+      <c r="C22" s="40" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="12"/>
-      <c r="E22" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="82">
+      <c r="E22" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="81">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="100"/>
-      <c r="B23" s="187"/>
+      <c r="A23" s="99"/>
+      <c r="B23" s="186"/>
       <c r="C23" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="48"/>
-      <c r="E23" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F23" s="82">
+      <c r="D23" s="47"/>
+      <c r="E23" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="81">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="100"/>
-      <c r="B24" s="187"/>
-      <c r="C24" s="41" t="s">
+      <c r="A24" s="99"/>
+      <c r="B24" s="186"/>
+      <c r="C24" s="40" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="9"/>
-      <c r="E24" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F24" s="82">
+      <c r="E24" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="81">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="100"/>
-      <c r="B25" s="187"/>
-      <c r="C25" s="41" t="s">
+      <c r="A25" s="99"/>
+      <c r="B25" s="186"/>
+      <c r="C25" s="40" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="82">
+      <c r="F25" s="81">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="125"/>
-      <c r="B26" s="188"/>
-      <c r="C26" s="41" t="s">
+      <c r="A26" s="124"/>
+      <c r="B26" s="187"/>
+      <c r="C26" s="40" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="12"/>
-      <c r="E26" s="140" t="s">
+      <c r="E26" s="139" t="s">
         <v>22</v>
       </c>
-      <c r="F26" s="82">
+      <c r="F26" s="81">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="102">
+      <c r="A27" s="101">
         <v>4</v>
       </c>
       <c r="B27" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="88" t="s">
+      <c r="C27" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="D27" s="56">
+      <c r="D27" s="55">
         <v>89</v>
       </c>
-      <c r="E27" s="56"/>
-      <c r="F27" s="89">
+      <c r="E27" s="55"/>
+      <c r="F27" s="88">
         <f>SUM(F28:F33)</f>
         <v>32</v>
       </c>
       <c r="J27" s="4"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="98"/>
-      <c r="B28" s="189" t="s">
+      <c r="A28" s="97"/>
+      <c r="B28" s="188" t="s">
         <v>101</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="34"/>
-      <c r="E28" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F28" s="77">
+      <c r="D28" s="33"/>
+      <c r="E28" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" s="76">
         <v>8</v>
       </c>
       <c r="J28" s="3"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="98"/>
-      <c r="B29" s="190"/>
+      <c r="A29" s="97"/>
+      <c r="B29" s="189"/>
       <c r="C29" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="34"/>
-      <c r="E29" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F29" s="77">
+      <c r="D29" s="33"/>
+      <c r="E29" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" s="76">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="98"/>
-      <c r="B30" s="190"/>
+      <c r="A30" s="97"/>
+      <c r="B30" s="189"/>
       <c r="C30" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="31"/>
+      <c r="D30" s="30"/>
       <c r="E30" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F30" s="77">
+      <c r="F30" s="76">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="98"/>
-      <c r="B31" s="190"/>
+      <c r="A31" s="97"/>
+      <c r="B31" s="189"/>
       <c r="C31" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D31" s="34"/>
-      <c r="E31" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F31" s="77">
+      <c r="D31" s="33"/>
+      <c r="E31" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" s="76">
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="98"/>
-      <c r="B32" s="190"/>
+      <c r="A32" s="97"/>
+      <c r="B32" s="189"/>
       <c r="C32" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F32" s="77">
+      <c r="D32" s="33"/>
+      <c r="E32" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="76">
         <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="128"/>
-      <c r="B33" s="191"/>
-      <c r="C33" s="61" t="s">
+      <c r="A33" s="127"/>
+      <c r="B33" s="190"/>
+      <c r="C33" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="42"/>
+      <c r="D33" s="41"/>
       <c r="E33" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F33" s="77">
+      <c r="F33" s="76">
         <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:11" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="103">
+      <c r="A34" s="102">
         <v>5</v>
       </c>
       <c r="B34" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="67" t="s">
+      <c r="C34" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="D34" s="65">
-        <v>3</v>
-      </c>
-      <c r="E34" s="58"/>
-      <c r="F34" s="85">
+      <c r="D34" s="64">
+        <v>3</v>
+      </c>
+      <c r="E34" s="57"/>
+      <c r="F34" s="84">
         <f>SUM(F35:F36)</f>
         <v>2.5</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="92"/>
-      <c r="B35" s="157" t="s">
+      <c r="A35" s="91"/>
+      <c r="B35" s="156" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="45" t="s">
+      <c r="C35" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="46"/>
+      <c r="D35" s="45"/>
       <c r="E35" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F35" s="81">
+      <c r="F35" s="80">
         <v>0.5</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="100"/>
-      <c r="B36" s="93"/>
-      <c r="C36" s="40" t="s">
+      <c r="A36" s="99"/>
+      <c r="B36" s="92"/>
+      <c r="C36" s="39" t="s">
         <v>30</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F36" s="82">
+      <c r="F36" s="81">
         <v>2</v>
       </c>
       <c r="I36" s="1"/>
       <c r="K36" s="1"/>
     </row>
     <row r="37" spans="1:11" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="97">
+      <c r="A37" s="96">
         <v>6</v>
       </c>
-      <c r="B37" s="131" t="s">
+      <c r="B37" s="130" t="s">
         <v>71</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D37" s="58">
+      <c r="D37" s="57">
         <v>5</v>
       </c>
-      <c r="E37" s="58"/>
-      <c r="F37" s="85">
+      <c r="E37" s="57"/>
+      <c r="F37" s="84">
         <f>SUM(F38:F40)</f>
         <v>9</v>
       </c>
@@ -4188,550 +4201,550 @@
       <c r="K37" s="6"/>
     </row>
     <row r="38" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="98"/>
-      <c r="B38" s="148" t="s">
+      <c r="A38" s="97"/>
+      <c r="B38" s="147" t="s">
         <v>103</v>
       </c>
-      <c r="C38" s="26" t="s">
+      <c r="C38" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D38" s="30"/>
-      <c r="E38" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F38" s="83"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F38" s="82"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="98"/>
-      <c r="B39" s="50"/>
+      <c r="A39" s="97"/>
+      <c r="B39" s="49"/>
       <c r="C39" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="38"/>
+      <c r="D39" s="37"/>
       <c r="E39" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F39" s="77">
+      <c r="F39" s="76">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="99"/>
+      <c r="A40" s="98"/>
       <c r="B40" s="16"/>
-      <c r="C40" s="39" t="s">
+      <c r="C40" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="D40" s="42"/>
-      <c r="E40" s="140" t="s">
+      <c r="D40" s="41"/>
+      <c r="E40" s="139" t="s">
         <v>22</v>
       </c>
-      <c r="F40" s="77">
+      <c r="F40" s="76">
         <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:11" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="104">
+      <c r="A41" s="103">
         <v>7</v>
       </c>
       <c r="B41" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="90" t="s">
+      <c r="C41" s="89" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="73">
-        <v>3</v>
-      </c>
-      <c r="E41" s="28"/>
-      <c r="F41" s="87">
+      <c r="D41" s="72">
+        <v>3</v>
+      </c>
+      <c r="E41" s="27"/>
+      <c r="F41" s="86">
         <f>SUM(F42:F46)</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="105"/>
-      <c r="B42" s="132" t="s">
+      <c r="A42" s="104"/>
+      <c r="B42" s="131" t="s">
         <v>85</v>
       </c>
-      <c r="C42" s="41" t="s">
+      <c r="C42" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="D42" s="48"/>
-      <c r="E42" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F42" s="81"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F42" s="80"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" s="92"/>
-      <c r="B43" s="94"/>
+      <c r="A43" s="91"/>
+      <c r="B43" s="93"/>
       <c r="C43" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D43" s="47"/>
-      <c r="E43" s="140" t="s">
+      <c r="D43" s="46"/>
+      <c r="E43" s="139" t="s">
         <v>22</v>
       </c>
-      <c r="F43" s="82"/>
+      <c r="F43" s="81"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A44" s="92"/>
+      <c r="A44" s="91"/>
       <c r="B44" s="7"/>
-      <c r="C44" s="45" t="s">
+      <c r="C44" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="D44" s="48"/>
-      <c r="E44" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F44" s="82"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F44" s="81"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="100"/>
-      <c r="B45" s="51"/>
-      <c r="C45" s="41" t="s">
+      <c r="A45" s="99"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="40" t="s">
         <v>39</v>
       </c>
       <c r="D45" s="9"/>
-      <c r="E45" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F45" s="82"/>
+      <c r="E45" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F45" s="81"/>
     </row>
     <row r="46" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="101"/>
+      <c r="A46" s="100"/>
       <c r="B46" s="7"/>
-      <c r="C46" s="45" t="s">
+      <c r="C46" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="D46" s="48"/>
-      <c r="E46" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F46" s="86">
+      <c r="D46" s="47"/>
+      <c r="E46" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F46" s="85">
         <v>0.5</v>
       </c>
     </row>
     <row r="47" spans="1:11" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A47" s="103">
+      <c r="A47" s="102">
         <v>8</v>
       </c>
       <c r="B47" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C47" s="90" t="s">
+      <c r="C47" s="89" t="s">
         <v>79</v>
       </c>
-      <c r="D47" s="44">
+      <c r="D47" s="43">
         <v>34</v>
       </c>
-      <c r="E47" s="44"/>
-      <c r="F47" s="91">
+      <c r="E47" s="43"/>
+      <c r="F47" s="90">
         <f>SUM(F48:F51)</f>
         <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:11" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="106"/>
-      <c r="B48" s="149" t="s">
+      <c r="A48" s="105"/>
+      <c r="B48" s="148" t="s">
         <v>104</v>
       </c>
       <c r="C48" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D48" s="66"/>
-      <c r="E48" s="140" t="s">
+      <c r="D48" s="65"/>
+      <c r="E48" s="139" t="s">
         <v>22</v>
       </c>
-      <c r="F48" s="84">
+      <c r="F48" s="83">
         <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:11" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="106"/>
-      <c r="B49" s="168" t="s">
+      <c r="A49" s="105"/>
+      <c r="B49" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="C49" s="141" t="s">
+      <c r="C49" s="140" t="s">
         <v>87</v>
       </c>
-      <c r="D49" s="63"/>
-      <c r="E49" s="138" t="s">
+      <c r="D49" s="62"/>
+      <c r="E49" s="137" t="s">
         <v>22</v>
       </c>
-      <c r="F49" s="84">
+      <c r="F49" s="83">
         <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A50" s="98"/>
-      <c r="B50" s="192"/>
+      <c r="A50" s="97"/>
+      <c r="B50" s="191"/>
       <c r="C50" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D50" s="34"/>
-      <c r="E50" s="138" t="s">
+      <c r="D50" s="33"/>
+      <c r="E50" s="137" t="s">
         <v>22</v>
       </c>
-      <c r="F50" s="77">
+      <c r="F50" s="76">
         <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:11" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="98"/>
-      <c r="B51" s="192"/>
-      <c r="C51" s="39" t="s">
+      <c r="A51" s="97"/>
+      <c r="B51" s="191"/>
+      <c r="C51" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="D51" s="31"/>
-      <c r="E51" s="140" t="s">
+      <c r="D51" s="30"/>
+      <c r="E51" s="139" t="s">
         <v>22</v>
       </c>
-      <c r="F51" s="77">
+      <c r="F51" s="76">
         <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="107">
+      <c r="A52" s="106">
         <v>9</v>
       </c>
-      <c r="B52" s="60" t="s">
+      <c r="B52" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="C52" s="133" t="s">
+      <c r="C52" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="D52" s="33">
+      <c r="D52" s="32">
         <v>8</v>
       </c>
-      <c r="E52" s="64"/>
-      <c r="F52" s="85">
+      <c r="E52" s="63"/>
+      <c r="F52" s="84">
         <f>SUM(F53:F55)</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:11" s="4" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="101"/>
-      <c r="B53" s="142" t="s">
+      <c r="A53" s="100"/>
+      <c r="B53" s="141" t="s">
         <v>94</v>
       </c>
-      <c r="C53" s="159" t="s">
+      <c r="C53" s="158" t="s">
         <v>93</v>
       </c>
-      <c r="D53" s="47"/>
-      <c r="E53" s="53" t="s">
+      <c r="D53" s="46"/>
+      <c r="E53" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="F53" s="82"/>
+      <c r="F53" s="81"/>
     </row>
     <row r="54" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="147"/>
-      <c r="B54" s="156" t="s">
+      <c r="A54" s="146"/>
+      <c r="B54" s="155" t="s">
         <v>100</v>
       </c>
       <c r="C54" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D54" s="146"/>
-      <c r="E54" s="53" t="s">
+      <c r="D54" s="145"/>
+      <c r="E54" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="F54" s="143"/>
+      <c r="F54" s="142"/>
     </row>
     <row r="55" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="144"/>
-      <c r="B55" s="62"/>
+      <c r="A55" s="143"/>
+      <c r="B55" s="61"/>
       <c r="C55" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D55" s="145"/>
-      <c r="E55" s="53" t="s">
+      <c r="D55" s="144"/>
+      <c r="E55" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="F55" s="143"/>
+      <c r="F55" s="142"/>
     </row>
     <row r="56" spans="1:11" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A56" s="95">
+      <c r="A56" s="94">
         <v>10</v>
       </c>
-      <c r="B56" s="59" t="s">
+      <c r="B56" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="C56" s="57" t="s">
+      <c r="C56" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="D56" s="28">
-        <v>3</v>
-      </c>
-      <c r="E56" s="64"/>
-      <c r="F56" s="85">
+      <c r="D56" s="27">
+        <v>3</v>
+      </c>
+      <c r="E56" s="63"/>
+      <c r="F56" s="84">
         <f>SUM(F57:F59)</f>
         <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A57" s="98"/>
-      <c r="B57" s="173" t="s">
+      <c r="A57" s="97"/>
+      <c r="B57" s="172" t="s">
         <v>97</v>
       </c>
       <c r="C57" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D57" s="31"/>
-      <c r="E57" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F57" s="77">
+      <c r="D57" s="30"/>
+      <c r="E57" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F57" s="76">
         <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="98"/>
-      <c r="B58" s="174"/>
+      <c r="A58" s="97"/>
+      <c r="B58" s="173"/>
       <c r="C58" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D58" s="34"/>
-      <c r="E58" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F58" s="77">
+      <c r="D58" s="33"/>
+      <c r="E58" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F58" s="76">
         <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="98"/>
-      <c r="B59" s="175"/>
-      <c r="C59" s="134" t="s">
+      <c r="A59" s="97"/>
+      <c r="B59" s="174"/>
+      <c r="C59" s="133" t="s">
         <v>42</v>
       </c>
-      <c r="D59" s="34"/>
-      <c r="E59" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F59" s="77">
+      <c r="D59" s="33"/>
+      <c r="E59" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F59" s="76">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A60" s="151">
+      <c r="A60" s="150">
         <v>11</v>
       </c>
-      <c r="B60" s="131" t="s">
+      <c r="B60" s="130" t="s">
         <v>107</v>
       </c>
-      <c r="C60" s="152" t="s">
+      <c r="C60" s="151" t="s">
         <v>43</v>
       </c>
-      <c r="D60" s="153">
+      <c r="D60" s="152">
         <v>0.5</v>
       </c>
-      <c r="E60" s="154"/>
-      <c r="F60" s="89">
+      <c r="E60" s="153"/>
+      <c r="F60" s="88">
         <f>SUM(F61)</f>
         <v>0.5</v>
       </c>
-      <c r="I60" s="155"/>
-      <c r="K60" s="155"/>
+      <c r="I60" s="154"/>
+      <c r="K60" s="154"/>
     </row>
     <row r="61" spans="1:11" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="100"/>
-      <c r="B61" s="158" t="s">
+      <c r="A61" s="99"/>
+      <c r="B61" s="157" t="s">
         <v>106</v>
       </c>
       <c r="C61" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D61" s="117"/>
-      <c r="E61" s="120" t="s">
-        <v>3</v>
-      </c>
-      <c r="F61" s="80">
+      <c r="D61" s="116"/>
+      <c r="E61" s="119" t="s">
+        <v>3</v>
+      </c>
+      <c r="F61" s="79">
         <v>0.5</v>
       </c>
       <c r="I61" s="6"/>
       <c r="K61" s="6"/>
     </row>
     <row r="62" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A62" s="97">
+      <c r="A62" s="96">
         <v>12</v>
       </c>
-      <c r="B62" s="150" t="s">
+      <c r="B62" s="149" t="s">
         <v>99</v>
       </c>
-      <c r="C62" s="57" t="s">
+      <c r="C62" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="D62" s="33">
+      <c r="D62" s="32">
         <v>2</v>
       </c>
-      <c r="E62" s="73"/>
-      <c r="F62" s="78">
+      <c r="E62" s="72"/>
+      <c r="F62" s="77">
         <f>SUM(F63)</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="98"/>
-      <c r="B63" s="130" t="s">
+      <c r="A63" s="97"/>
+      <c r="B63" s="129" t="s">
         <v>90</v>
       </c>
       <c r="C63" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D63" s="122"/>
-      <c r="E63" s="118" t="s">
-        <v>3</v>
-      </c>
-      <c r="F63" s="123">
+      <c r="D63" s="121"/>
+      <c r="E63" s="117" t="s">
+        <v>3</v>
+      </c>
+      <c r="F63" s="122">
         <v>0.5</v>
       </c>
     </row>
     <row r="64" spans="1:11" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A64" s="97">
+      <c r="A64" s="96">
         <v>13</v>
       </c>
-      <c r="B64" s="68" t="s">
+      <c r="B64" s="67" t="s">
         <v>108</v>
       </c>
-      <c r="C64" s="27" t="s">
+      <c r="C64" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="D64" s="43">
+      <c r="D64" s="42">
         <v>8</v>
       </c>
-      <c r="E64" s="65"/>
-      <c r="F64" s="85">
+      <c r="E64" s="64"/>
+      <c r="F64" s="84">
         <f>SUM(F65:F66)</f>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:12" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="100"/>
-      <c r="B65" s="176" t="s">
+      <c r="A65" s="99"/>
+      <c r="B65" s="175" t="s">
         <v>109</v>
       </c>
       <c r="C65" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D65" s="46"/>
-      <c r="E65" s="138" t="s">
+      <c r="D65" s="45"/>
+      <c r="E65" s="137" t="s">
         <v>22</v>
       </c>
-      <c r="F65" s="82"/>
+      <c r="F65" s="81"/>
       <c r="L65" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:12" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="125"/>
-      <c r="B66" s="177"/>
-      <c r="C66" s="52" t="s">
+      <c r="A66" s="124"/>
+      <c r="B66" s="176"/>
+      <c r="C66" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="D66" s="54"/>
-      <c r="E66" s="139" t="s">
+      <c r="D66" s="53"/>
+      <c r="E66" s="138" t="s">
         <v>22</v>
       </c>
-      <c r="F66" s="126"/>
+      <c r="F66" s="125"/>
     </row>
     <row r="67" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A67" s="103">
+      <c r="A67" s="102">
         <v>14</v>
       </c>
       <c r="B67" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C67" s="170" t="s">
+      <c r="C67" s="169" t="s">
         <v>82</v>
       </c>
-      <c r="D67" s="73">
+      <c r="D67" s="72">
         <v>1</v>
       </c>
-      <c r="E67" s="65"/>
-      <c r="F67" s="85">
+      <c r="E67" s="64"/>
+      <c r="F67" s="84">
         <f>SUM(F68:F69)</f>
         <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A68" s="98"/>
-      <c r="B68" s="178" t="s">
+      <c r="A68" s="97"/>
+      <c r="B68" s="177" t="s">
         <v>69</v>
       </c>
       <c r="C68" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D68" s="30"/>
-      <c r="E68" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F68" s="77">
+      <c r="D68" s="29"/>
+      <c r="E68" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F68" s="76">
         <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="128"/>
-      <c r="B69" s="179"/>
-      <c r="C69" s="129" t="s">
+      <c r="A69" s="127"/>
+      <c r="B69" s="178"/>
+      <c r="C69" s="128" t="s">
         <v>50</v>
       </c>
-      <c r="D69" s="49"/>
+      <c r="D69" s="48"/>
       <c r="E69" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F69" s="127">
+      <c r="F69" s="126">
         <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:12" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="169">
+      <c r="A70" s="168">
         <v>15</v>
       </c>
       <c r="B70" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C70" s="133" t="s">
+      <c r="C70" s="132" t="s">
         <v>52</v>
       </c>
-      <c r="D70" s="28">
-        <v>3</v>
-      </c>
-      <c r="E70" s="44"/>
-      <c r="F70" s="87">
+      <c r="D70" s="27">
+        <v>3</v>
+      </c>
+      <c r="E70" s="43"/>
+      <c r="F70" s="86">
         <f>SUM(F71:F72)</f>
         <v>1.5</v>
       </c>
       <c r="H70"/>
     </row>
     <row r="71" spans="1:12" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A71" s="160"/>
-      <c r="B71" s="132" t="s">
+      <c r="A71" s="159"/>
+      <c r="B71" s="131" t="s">
         <v>112</v>
       </c>
-      <c r="C71" s="161" t="s">
+      <c r="C71" s="160" t="s">
         <v>110</v>
       </c>
-      <c r="D71" s="146"/>
-      <c r="E71" s="166" t="s">
+      <c r="D71" s="145"/>
+      <c r="E71" s="165" t="s">
         <v>1</v>
       </c>
-      <c r="F71" s="162">
+      <c r="F71" s="161">
         <v>0.5</v>
       </c>
       <c r="H71"/>
     </row>
     <row r="72" spans="1:12" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="163"/>
-      <c r="B72" s="171"/>
-      <c r="C72" s="165" t="s">
+      <c r="A72" s="162"/>
+      <c r="B72" s="170"/>
+      <c r="C72" s="164" t="s">
         <v>111</v>
       </c>
-      <c r="D72" s="172"/>
-      <c r="E72" s="167" t="s">
+      <c r="D72" s="171"/>
+      <c r="E72" s="166" t="s">
         <v>1</v>
       </c>
-      <c r="F72" s="164">
+      <c r="F72" s="163">
         <v>1</v>
       </c>
       <c r="H72"/>
@@ -4758,23 +4771,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="31266629-21bd-4ff6-9695-79f97710c305" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E4167577FDD28A44889000E11502BE52" ma:contentTypeVersion="14" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="fc7dd6c0c9e419aea3cd89e5917a0267">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="31266629-21bd-4ff6-9695-79f97710c305" xmlns:ns4="7371320f-86a8-4db4-b1f9-dce78a203d2a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="142e0f016e20ee8e5e9578fc7f0f5d6b" ns3:_="" ns4:_="">
     <xsd:import namespace="31266629-21bd-4ff6-9695-79f97710c305"/>
@@ -5001,10 +4997,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="31266629-21bd-4ff6-9695-79f97710c305" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15760DDD-D48D-4232-962A-D4D301C87DE7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{233F6942-0BB8-4AA8-8651-03B35DC38943}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="31266629-21bd-4ff6-9695-79f97710c305"/>
+    <ds:schemaRef ds:uri="7371320f-86a8-4db4-b1f9-dce78a203d2a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5027,20 +5051,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{233F6942-0BB8-4AA8-8651-03B35DC38943}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15760DDD-D48D-4232-962A-D4D301C87DE7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="31266629-21bd-4ff6-9695-79f97710c305"/>
-    <ds:schemaRef ds:uri="7371320f-86a8-4db4-b1f9-dce78a203d2a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>